<commit_message>
smv vv: update smoke test spreadsheet
</commit_message>
<xml_diff>
--- a/smv/smoketest/smoke_test.xlsx
+++ b/smv/smoketest/smoke_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gforney\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gforney\FireModels_fork\fig\smv\smoketest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743C5ABC-F1A2-4F17-B540-1BDB44BBAEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0880246-BD7B-423C-976D-AD20E0697BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4068" yWindow="3024" windowWidth="23040" windowHeight="13512" xr2:uid="{0A9ECB99-2F97-4588-B4A3-75BD2571C6D4}"/>
+    <workbookView xWindow="864" yWindow="3036" windowWidth="27984" windowHeight="16104" xr2:uid="{0A9ECB99-2F97-4588-B4A3-75BD2571C6D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
     <t>grey level</t>
   </si>
   <si>
-    <t>soot mass fraction</t>
-  </si>
-  <si>
-    <t>soot density</t>
-  </si>
-  <si>
     <t>old path length</t>
   </si>
   <si>
@@ -93,14 +87,28 @@
   </si>
   <si>
     <t>dx</t>
+  </si>
+  <si>
+    <t>soot mass fraction(fds input)</t>
+  </si>
+  <si>
+    <t>soot density(compute alpha)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,13 +456,14 @@
   <dimension ref="C2:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="5" max="6" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
     <col min="8" max="9" width="15.33203125" customWidth="1"/>
     <col min="10" max="10" width="16.5546875" customWidth="1"/>
   </cols>
@@ -463,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="3:12" x14ac:dyDescent="0.3">
@@ -481,10 +491,10 @@
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -505,13 +515,13 @@
         <f>E5/1.195</f>
         <v>1.8007855704714752E-4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>100</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>0.5</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>8700</v>
       </c>
     </row>
@@ -521,7 +531,7 @@
         <v>0.39215686274509803</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.3">
@@ -546,23 +556,25 @@
         <v>5.8983088765212361</v>
       </c>
       <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
         <v>8</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>9</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="H9">
+        <f>H5</f>
         <v>0.5</v>
       </c>
       <c r="I9">
+        <f>G5</f>
         <v>100</v>
       </c>
       <c r="J9">
@@ -576,18 +588,18 @@
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
         <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <f>INT(E8)</f>
@@ -604,7 +616,7 @@
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <f>D11/255</f>
@@ -643,5 +655,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>